<commit_message>
Modification du code mainwindow.py: => modif de l'affichage des détails prospect dans le text edit
</commit_message>
<xml_diff>
--- a/src/main/resources/base/liste_Pros_occ.xlsx
+++ b/src/main/resources/base/liste_Pros_occ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imaf/pro_occitans/src/main/resources/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A423D8E-9BCF-4840-80C2-33E0B9389F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C837BF3-4232-1A47-843C-7EA1D7CAD91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="1660" windowWidth="16420" windowHeight="17440" xr2:uid="{0605DF22-7999-184D-A11E-3A59B118BED7}"/>
   </bookViews>
@@ -550,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376B3740-3729-DD4F-AFA5-A0EC8C8F4E6A}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A18" sqref="A18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,6 +749,12 @@
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ajout de commentaires préparation d'une nouvelle fonction créer des événements calendrier avec le module ics
</commit_message>
<xml_diff>
--- a/src/main/resources/base/liste_Pros_occ.xlsx
+++ b/src/main/resources/base/liste_Pros_occ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imaf/pro_occitans/src/main/resources/base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imaf/my_python_projects/pro_occitans/src/main/resources/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C837BF3-4232-1A47-843C-7EA1D7CAD91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876D2DEF-80D7-A14F-B602-59721AFCA410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="1660" windowWidth="16420" windowHeight="17440" xr2:uid="{0605DF22-7999-184D-A11E-3A59B118BED7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Action Clim</t>
   </si>
@@ -187,6 +187,21 @@
   </si>
   <si>
     <t>0684088720</t>
+  </si>
+  <si>
+    <t>De716</t>
+  </si>
+  <si>
+    <t>tinoveler@gmail.com</t>
+  </si>
+  <si>
+    <t>0650591900</t>
+  </si>
+  <si>
+    <t>COT</t>
+  </si>
+  <si>
+    <t>enaccf31400@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -553,7 +568,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C19"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,10 +766,26 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -762,6 +793,7 @@
     <hyperlink ref="B4" r:id="rId2" xr:uid="{3EBB8367-0631-B64C-ADB6-82CA715B035B}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{22A0A164-91CC-D146-8277-5BAB9567C864}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{5B5EA812-E593-474A-BD02-E3F5A61E2C84}"/>
+    <hyperlink ref="B19" r:id="rId5" xr:uid="{43BC190F-B3D0-E248-AE8F-7D03A907D4DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>